<commit_message>
Changed secretary on timesheet
</commit_message>
<xml_diff>
--- a/timesheets/week2.xlsx
+++ b/timesheets/week2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Documents/team-project/timesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EE7A8A-2E59-BB41-81F5-B679D9A8EC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B03CF-EF57-EE44-A7A5-A0689C29D159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="28480" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14480" yWindow="500" windowWidth="14160" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Timesheet" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>Creating Personas</t>
   </si>
   <si>
-    <t>Harsh</t>
+    <t>Ethan</t>
   </si>
 </sst>
 </file>
@@ -303,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -349,78 +349,77 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,7 +743,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -773,14 +772,14 @@
     </row>
     <row r="2" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="31" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="31"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -789,14 +788,14 @@
     </row>
     <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="29"/>
+      <c r="E3" s="39"/>
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -804,19 +803,19 @@
     </row>
     <row r="4" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="39"/>
       <c r="G4" s="2"/>
       <c r="H4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="21">
         <v>45313</v>
       </c>
       <c r="J4" s="1"/>
@@ -827,16 +826,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="32">
+      <c r="D5" s="48">
         <v>45321</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="22">
         <v>45321</v>
       </c>
       <c r="J5" s="1"/>
@@ -855,12 +854,12 @@
     </row>
     <row r="7" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5"/>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
@@ -877,12 +876,12 @@
     </row>
     <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="13">
         <v>45313</v>
       </c>
@@ -900,12 +899,12 @@
     </row>
     <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="13">
         <v>45314</v>
       </c>
@@ -923,12 +922,12 @@
     </row>
     <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="13">
         <v>45317</v>
       </c>
@@ -939,19 +938,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="I10" s="16">
-        <f t="shared" ref="I10:I14" si="0">(H10-G10)*24</f>
+        <f t="shared" ref="I10:I12" si="0">(H10-G10)*24</f>
         <v>0.49999999999999822</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="13">
         <v>45320</v>
       </c>
@@ -975,16 +974,16 @@
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
       <c r="E12" s="46"/>
-      <c r="F12" s="47">
+      <c r="F12" s="29">
         <v>45321</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="30">
         <v>0.5</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H12" s="31">
         <v>0.54166666666666663</v>
       </c>
-      <c r="I12" s="50">
+      <c r="I12" s="32">
         <f t="shared" si="0"/>
         <v>0.99999999999999911</v>
       </c>
@@ -992,28 +991,28 @@
     </row>
     <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="42" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="28">
         <f>SUM(I8:I12)</f>
         <v>4.9999999999999982</v>
       </c>
@@ -1040,15 +1039,15 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="41"/>
+      <c r="I16" s="26"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
       <c r="B17" s="4"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="10"/>
       <c r="G17" s="5"/>
       <c r="H17" s="3"/>

</xml_diff>